<commit_message>
Start Time added, App Auth integrated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisRamos\OneDrive - Roboyo Global\Documents\UiPath\Personal\BotMonitor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6344BF00-2426-4290-883B-A23BC0FF6F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE505BE-443C-401B-827E-C2CCA449058E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="105">
   <si>
     <t>Name</t>
   </si>
@@ -271,57 +271,6 @@
     <t>Other Constants</t>
   </si>
   <si>
-    <t>Platform</t>
-  </si>
-  <si>
-    <t>UsePlatform</t>
-  </si>
-  <si>
-    <t>If true, the bot will perform all the Platform activities</t>
-  </si>
-  <si>
-    <t>RaiseTicketPerFailedTransaction</t>
-  </si>
-  <si>
-    <t>PlatformURL</t>
-  </si>
-  <si>
-    <t>Platform URL where all the data will be uploaded</t>
-  </si>
-  <si>
-    <t>PlatformProcessID</t>
-  </si>
-  <si>
-    <t>PlatformProcessID given by the Platform Admin</t>
-  </si>
-  <si>
-    <t>AMSAgentId</t>
-  </si>
-  <si>
-    <t>ID for the asigned AMS agent</t>
-  </si>
-  <si>
-    <t>FreshdeskToken</t>
-  </si>
-  <si>
-    <t>Asset that stores the Beecker's Freshdesk Token</t>
-  </si>
-  <si>
-    <t>PlatformAPICredentials</t>
-  </si>
-  <si>
-    <t>Asset that stores the Beecker's API Dashboard Credentials</t>
-  </si>
-  <si>
-    <t>UploadDataPerTransaction</t>
-  </si>
-  <si>
-    <t>If true, the bot will raise a ticket per failed transaction</t>
-  </si>
-  <si>
-    <t>If true, the bot will upload the data pereach transaction</t>
-  </si>
-  <si>
     <t>TransactionData excel file path</t>
   </si>
   <si>
@@ -355,24 +304,12 @@
     <t>The column letter where the TicketId is setted</t>
   </si>
   <si>
-    <t>RaiseFinalTicket</t>
-  </si>
-  <si>
-    <t>If true, the bot will raise a ticket at the EndProcess</t>
-  </si>
-  <si>
     <t>bots@beecker.ai</t>
   </si>
   <si>
-    <t>Plat_TecM_Dev</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>TemplateReportPath</t>
   </si>
   <si>
@@ -394,7 +331,13 @@
     <t>G</t>
   </si>
   <si>
-    <t>F</t>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Reporting</t>
   </si>
 </sst>
 </file>
@@ -535,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -549,15 +492,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -587,9 +521,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -908,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -955,68 +886,68 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1024,11 +955,11 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2013,10 +1944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2062,11 +1993,11 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2161,13 +2092,13 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2195,13 +2126,13 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2243,7 +2174,7 @@
         <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>52</v>
@@ -2287,7 +2218,7 @@
         <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>62</v>
@@ -2342,7 +2273,7 @@
         <v>71</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>72</v>
@@ -2383,11 +2314,11 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2545,126 +2476,59 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A32" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
+      <c r="A32" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="4" t="b">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="4" t="b">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="B34" t="s">
+        <v>102</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="4" t="b">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="B35" t="s">
+        <v>103</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B36" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="5">
-        <v>91</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="5">
-        <v>73000820867</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B40" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B41" t="s">
-        <v>123</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B42" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" s="18" t="s">
+      <c r="A36" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-    </row>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3621,30 +3485,20 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
-    <row r="1004" ht="14.25" customHeight="1"/>
-    <row r="1005" ht="14.25" customHeight="1"/>
-    <row r="1006" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A36:C36"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{AF0B567B-318D-49F7-BF47-37075073F103}">
       <formula1>"dd-MM-yyyy,MM-yyyy"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31 B33:B36" xr:uid="{248F42FF-649C-43CB-A4E9-5F8C8224B40B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31" xr:uid="{248F42FF-649C-43CB-A4E9-5F8C8224B40B}">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37" xr:uid="{4F91D44E-DA38-4C59-B42F-D8C0EF8BBE54}">
-      <formula1>"https://dev.api.dashboard.beecker.ai/,https://api.dashboard.beecker.ai/"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3653,10 +3507,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3703,40 +3557,10 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4728,15 +4552,7 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A5:D5"/>
-  </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4744,10 +4560,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D414877D-0A7D-4040-A170-961E96460DE7}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4771,51 +4587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A6:D6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>